<commit_message>
adds metadata fields information, for those available
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_snorkel_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\edi-feather-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288A61C9-2175-4FBE-B05A-BD39841734AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F390420-BA1E-4B8E-91F5-3835DE8E3DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4030" yWindow="890" windowWidth="18240" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="70">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -202,9 +202,6 @@
     <t xml:space="preserve">Substrate description from survey location </t>
   </si>
   <si>
-    <t xml:space="preserve">Instream cover from survey location </t>
-  </si>
-  <si>
     <t>Features of stream</t>
   </si>
   <si>
@@ -216,13 +213,37 @@
   <si>
     <t xml:space="preserve">If fish fin is clipped </t>
   </si>
+  <si>
+    <t>Location were seine data was collected</t>
+  </si>
+  <si>
+    <t>Time when water temperature was collected</t>
+  </si>
+  <si>
+    <t>Time when snorkel survey started</t>
+  </si>
+  <si>
+    <t>Number of fish observed</t>
+  </si>
+  <si>
+    <t>whole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instream cover at survey location </t>
+  </si>
+  <si>
+    <t>Overhead cover at survey location</t>
+  </si>
+  <si>
+    <t>Depth on water in meters</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -307,15 +328,17 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="22" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,8 +557,8 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -609,7 +632,7 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="1"/>
@@ -639,10 +662,10 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="1"/>
@@ -671,7 +694,7 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -690,8 +713,12 @@
       <c r="I4" s="2"/>
       <c r="J4" s="3"/>
       <c r="K4" s="10"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
+      <c r="L4" s="11">
+        <v>0</v>
+      </c>
+      <c r="M4" s="15">
+        <v>8000</v>
+      </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -707,10 +734,10 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="1"/>
@@ -739,10 +766,10 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -762,8 +789,12 @@
       <c r="I6" s="2"/>
       <c r="J6" s="5"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="3"/>
+      <c r="L6" s="14">
+        <v>0</v>
+      </c>
+      <c r="M6" s="14">
+        <v>4</v>
+      </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -779,10 +810,10 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="12" t="s">
         <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -821,10 +852,12 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="13" t="s">
+        <v>63</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="2"/>
       <c r="E8" s="1"/>
@@ -851,10 +884,12 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="13" t="s">
+        <v>64</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
       <c r="E9" s="1"/>
@@ -881,10 +916,12 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="13" t="s">
+        <v>64</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="2"/>
       <c r="E10" s="1"/>
@@ -911,10 +948,12 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="13" t="s">
+        <v>62</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
       <c r="E11" s="1"/>
@@ -941,7 +980,7 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="1"/>
@@ -971,7 +1010,7 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="1"/>
@@ -1001,7 +1040,7 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B14" s="1"/>
@@ -1014,8 +1053,8 @@
       <c r="I14" s="2"/>
       <c r="J14" s="5"/>
       <c r="K14" s="6"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1031,7 +1070,7 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="12" t="s">
         <v>36</v>
       </c>
       <c r="B15" s="1"/>
@@ -1044,7 +1083,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
-      <c r="L15" s="12"/>
+      <c r="L15" s="11"/>
       <c r="M15" s="3"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -1061,21 +1100,35 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="3"/>
+      <c r="E16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="I16" s="2"/>
       <c r="J16" s="5"/>
       <c r="K16" s="6"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="3"/>
+      <c r="L16" s="11">
+        <v>0</v>
+      </c>
+      <c r="M16" s="3">
+        <v>25000</v>
+      </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -1091,7 +1144,7 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="1"/>
@@ -1121,7 +1174,7 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="12" t="s">
         <v>39</v>
       </c>
       <c r="B18" s="1"/>
@@ -1134,8 +1187,12 @@
       <c r="I18" s="2"/>
       <c r="J18" s="3"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
+      <c r="L18" s="3">
+        <v>0</v>
+      </c>
+      <c r="M18" s="3">
+        <v>950</v>
+      </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -1151,10 +1208,10 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1187,11 +1244,11 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="14" t="s">
-        <v>58</v>
+      <c r="B20" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>13</v>
@@ -1223,13 +1280,19 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D21" s="2"/>
-      <c r="E21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -1253,11 +1316,11 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>59</v>
+      <c r="B22" s="12" t="s">
+        <v>58</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>13</v>
@@ -1289,21 +1352,35 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="3"/>
+      <c r="E23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
+      <c r="H23" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="I23" s="2"/>
       <c r="J23" s="3"/>
       <c r="K23" s="2"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
+      <c r="L23" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="M23" s="14">
+        <v>3</v>
+      </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -1319,7 +1396,7 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="12" t="s">
         <v>45</v>
       </c>
       <c r="B24" s="1"/>
@@ -1349,7 +1426,7 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="12" t="s">
         <v>46</v>
       </c>
       <c r="B25" s="1"/>
@@ -1379,11 +1456,11 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="14" t="s">
-        <v>60</v>
+      <c r="B26" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>13</v>
@@ -1415,11 +1492,11 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="14" t="s">
-        <v>61</v>
+      <c r="B27" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>13</v>
@@ -1451,11 +1528,11 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="12" t="s">
         <v>49</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
adds field descriptions to metadata xlsx
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_snorkel_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\edi-feather-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778AC8FB-5482-486E-8BDD-16898FE74D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC359CCD-2187-444E-B848-D3C6E756C5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7720" yWindow="2340" windowWidth="16070" windowHeight="12250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17580" yWindow="1530" windowWidth="16065" windowHeight="12255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="83">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -246,13 +246,44 @@
   <si>
     <t>section_number</t>
   </si>
+  <si>
+    <t>dateTime</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>ask liz</t>
+  </si>
+  <si>
+    <t>Fish species</t>
+  </si>
+  <si>
+    <t>Fork length of juvenile</t>
+  </si>
+  <si>
+    <t>millimeter</t>
+  </si>
+  <si>
+    <t>Distance from the bank</t>
+  </si>
+  <si>
+    <t>meter</t>
+  </si>
+  <si>
+    <t>check with liz</t>
+  </si>
+  <si>
+    <t>Identification number of survey</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -313,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -342,6 +373,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -562,8 +599,8 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -640,7 +677,9 @@
       <c r="A2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="14" t="s">
+        <v>82</v>
+      </c>
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
@@ -745,9 +784,13 @@
       <c r="B5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -863,9 +906,13 @@
       <c r="B8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -895,9 +942,13 @@
       <c r="B9" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -929,7 +980,9 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -956,7 +1009,9 @@
       <c r="A11" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
       <c r="E11" s="1"/>
@@ -986,7 +1041,9 @@
       <c r="A12" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
       <c r="E12" s="1"/>
@@ -1060,7 +1117,9 @@
       <c r="A14" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
       <c r="E14" s="1"/>
@@ -1090,7 +1149,9 @@
       <c r="A15" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
       <c r="E15" s="1"/>
@@ -1256,7 +1317,7 @@
         <v>0.05</v>
       </c>
       <c r="M19" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -1384,7 +1445,7 @@
       <c r="A23" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="14" t="s">
         <v>59</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -1420,10 +1481,14 @@
       <c r="A24" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="12" t="s">
+        <v>61</v>
+      </c>
       <c r="C24" s="1"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -1510,10 +1575,14 @@
       <c r="A27" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="C27" s="1"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -1540,18 +1609,34 @@
       <c r="A28" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="B28" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D28" s="2"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
+      <c r="E28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="I28" s="2"/>
       <c r="J28" s="3"/>
       <c r="K28" s="2"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
+      <c r="L28" s="3">
+        <v>0</v>
+      </c>
+      <c r="M28" s="3">
+        <v>900</v>
+      </c>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -1570,18 +1655,34 @@
       <c r="A29" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="B29" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D29" s="2"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
+      <c r="E29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="I29" s="2"/>
       <c r="J29" s="3"/>
       <c r="K29" s="2"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
+      <c r="L29" s="3">
+        <v>0</v>
+      </c>
+      <c r="M29" s="3">
+        <v>10</v>
+      </c>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
@@ -1600,7 +1701,9 @@
       <c r="A30" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
       <c r="E30" s="1"/>
@@ -1631,17 +1734,29 @@
         <v>71</v>
       </c>
       <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D31" s="2"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="3"/>
+      <c r="E31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
+      <c r="H31" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="I31" s="2"/>
       <c r="J31" s="3"/>
       <c r="K31" s="2"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
+      <c r="L31" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="M31" s="17">
+        <v>9</v>
+      </c>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
@@ -1660,18 +1775,32 @@
       <c r="A32" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D32" s="2"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="3"/>
+      <c r="E32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
+      <c r="H32" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="I32" s="2"/>
       <c r="J32" s="3"/>
       <c r="K32" s="2"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
+      <c r="L32" s="3">
+        <v>4</v>
+      </c>
+      <c r="M32" s="3">
+        <v>36</v>
+      </c>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>

</xml_diff>

<commit_message>
addresses TODOs, marks fields that need meaning confirmation
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_snorkel_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\edi-feather-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC359CCD-2187-444E-B848-D3C6E756C5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AEB854-A923-4801-B91A-7A636980183C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17580" yWindow="1530" windowWidth="16065" windowHeight="12255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2760" yWindow="520" windowWidth="19080" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="83">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -253,9 +253,6 @@
     <t>?</t>
   </si>
   <si>
-    <t>ask liz</t>
-  </si>
-  <si>
     <t>Fish species</t>
   </si>
   <si>
@@ -271,10 +268,13 @@
     <t>meter</t>
   </si>
   <si>
-    <t>check with liz</t>
+    <t>Identification number of survey</t>
   </si>
   <si>
-    <t>Identification number of survey</t>
+    <t>Number of map section from DMP</t>
+  </si>
+  <si>
+    <t>Fish size classification</t>
   </si>
 </sst>
 </file>
@@ -344,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -375,9 +375,6 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -599,8 +596,8 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -677,12 +674,14 @@
       <c r="A2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>82</v>
+      <c r="B2" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -714,7 +713,9 @@
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -1073,7 +1074,7 @@
       <c r="A13" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1118,11 +1119,15 @@
         <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1293,7 +1298,7 @@
       <c r="A19" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1445,7 +1450,7 @@
       <c r="A23" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -1515,7 +1520,9 @@
       <c r="A25" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="C25" s="1"/>
       <c r="D25" s="2"/>
       <c r="E25" s="1"/>
@@ -1545,7 +1552,9 @@
       <c r="A26" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="C26" s="1"/>
       <c r="D26" s="2"/>
       <c r="E26" s="1"/>
@@ -1576,7 +1585,7 @@
         <v>67</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="2"/>
@@ -1609,8 +1618,8 @@
       <c r="A28" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="15" t="s">
-        <v>77</v>
+      <c r="B28" s="12" t="s">
+        <v>76</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>15</v>
@@ -1622,8 +1631,8 @@
       <c r="F28" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G28" s="16" t="s">
-        <v>78</v>
+      <c r="G28" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>57</v>
@@ -1655,8 +1664,8 @@
       <c r="A29" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="14" t="s">
-        <v>79</v>
+      <c r="B29" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>15</v>
@@ -1669,7 +1678,7 @@
         <v>15</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>17</v>
@@ -1733,7 +1742,9 @@
       <c r="A31" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="C31" s="1" t="s">
         <v>15</v>
       </c>
@@ -1751,10 +1762,10 @@
       <c r="I31" s="2"/>
       <c r="J31" s="3"/>
       <c r="K31" s="2"/>
-      <c r="L31" s="17">
+      <c r="L31" s="14">
         <v>0.5</v>
       </c>
-      <c r="M31" s="17">
+      <c r="M31" s="14">
         <v>9</v>
       </c>
       <c r="N31" s="1"/>

</xml_diff>

<commit_message>
adds field types and attribute labels to metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_snorkel_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\edi-feather-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AEB854-A923-4801-B91A-7A636980183C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA5AB7D-4B82-4419-831E-E518F8444A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="520" windowWidth="19080" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="86">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -276,14 +276,24 @@
   <si>
     <t>Fish size classification</t>
   </si>
+  <si>
+    <t>ordinal</t>
+  </si>
+  <si>
+    <t>snorkel_survey</t>
+  </si>
+  <si>
+    <t>cubicFeetPerSecond</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -344,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -376,6 +386,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -595,9 +615,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -677,19 +697,31 @@
       <c r="B2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2"/>
+      <c r="C2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="15" t="s">
+        <v>44</v>
+      </c>
       <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="I2" s="2"/>
       <c r="J2" s="5"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="3"/>
+      <c r="L2" s="17">
+        <v>2</v>
+      </c>
+      <c r="M2" s="3">
+        <v>581</v>
+      </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -712,7 +744,9 @@
         <v>47</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>73</v>
       </c>
@@ -748,12 +782,18 @@
       <c r="C4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>85</v>
+      </c>
       <c r="H4" s="3"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3"/>
@@ -762,7 +802,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="3">
-        <v>8000</v>
+        <v>9564</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -788,7 +828,9 @@
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
@@ -824,7 +866,9 @@
       <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E6" s="1" t="s">
         <v>16</v>
       </c>
@@ -866,14 +910,16 @@
         <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>15</v>
+      <c r="F7" s="15" t="s">
+        <v>44</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>46</v>
@@ -884,8 +930,12 @@
       <c r="I7" s="2"/>
       <c r="J7" s="5"/>
       <c r="K7" s="6"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="3"/>
+      <c r="L7" s="18">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3">
+        <v>21.67</v>
+      </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -910,7 +960,9 @@
       <c r="C8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E8" s="1" t="s">
         <v>73</v>
       </c>
@@ -946,7 +998,9 @@
       <c r="C9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E9" s="1" t="s">
         <v>73</v>
       </c>
@@ -979,8 +1033,12 @@
       <c r="B10" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1013,9 +1071,15 @@
       <c r="B11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1045,9 +1109,15 @@
       <c r="B12" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1080,7 +1150,9 @@
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1097,8 +1169,8 @@
       <c r="L13" s="11">
         <v>0</v>
       </c>
-      <c r="M13" s="3">
-        <v>25000</v>
+      <c r="M13" s="16">
+        <v>30000</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1124,7 +1196,9 @@
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1157,19 +1231,29 @@
       <c r="B15" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="3"/>
+      <c r="C15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="I15" s="2"/>
       <c r="J15" s="3"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="3">
+      <c r="L15" s="16">
         <v>0</v>
       </c>
-      <c r="M15" s="3">
+      <c r="M15" s="16">
         <v>950</v>
       </c>
       <c r="N15" s="1"/>
@@ -1196,7 +1280,9 @@
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1232,7 +1318,9 @@
       <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1268,7 +1356,9 @@
       <c r="C18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E18" s="1" t="s">
         <v>14</v>
       </c>
@@ -1304,7 +1394,9 @@
       <c r="C19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1346,9 +1438,11 @@
         <v>52</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E20" s="1" t="s">
         <v>14</v>
       </c>
@@ -1384,7 +1478,9 @@
       <c r="C21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E21" s="1" t="s">
         <v>14</v>
       </c>
@@ -1420,7 +1516,9 @@
       <c r="C22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E22" s="1" t="s">
         <v>14</v>
       </c>
@@ -1456,7 +1554,9 @@
       <c r="C23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E23" s="1" t="s">
         <v>14</v>
       </c>
@@ -1489,8 +1589,12 @@
       <c r="B24" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
+      <c r="C24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E24" s="1" t="s">
         <v>14</v>
       </c>
@@ -1523,9 +1627,15 @@
       <c r="B25" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -1555,9 +1665,15 @@
       <c r="B26" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="1"/>
+      <c r="C26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -1587,8 +1703,12 @@
       <c r="B27" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="2"/>
+      <c r="C27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E27" s="1" t="s">
         <v>14</v>
       </c>
@@ -1624,7 +1744,9 @@
       <c r="C28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E28" s="1" t="s">
         <v>16</v>
       </c>
@@ -1670,7 +1792,9 @@
       <c r="C29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="2"/>
+      <c r="D29" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E29" s="1" t="s">
         <v>16</v>
       </c>
@@ -1686,10 +1810,10 @@
       <c r="I29" s="2"/>
       <c r="J29" s="3"/>
       <c r="K29" s="2"/>
-      <c r="L29" s="3">
+      <c r="L29" s="14">
         <v>0</v>
       </c>
-      <c r="M29" s="3">
+      <c r="M29" s="14">
         <v>10</v>
       </c>
       <c r="N29" s="1"/>
@@ -1713,9 +1837,15 @@
       <c r="B30" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -1748,7 +1878,9 @@
       <c r="C31" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E31" s="1" t="s">
         <v>16</v>
       </c>
@@ -1792,7 +1924,9 @@
       <c r="C32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="2"/>
+      <c r="D32" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E32" s="1" t="s">
         <v>16</v>
       </c>
@@ -1806,11 +1940,11 @@
       <c r="I32" s="2"/>
       <c r="J32" s="3"/>
       <c r="K32" s="2"/>
-      <c r="L32" s="3">
-        <v>4</v>
+      <c r="L32" s="14">
+        <v>1</v>
       </c>
-      <c r="M32" s="3">
-        <v>36</v>
+      <c r="M32" s="14">
+        <v>20</v>
       </c>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>

</xml_diff>

<commit_message>
adds costum units definitions
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_snorkel_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\edi-feather-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5E9931-8E48-426F-907B-6EEA3A949F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED5C50C-44B4-4CA6-8ABC-8DC142114FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="93">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -297,15 +297,25 @@
   <si>
     <t>none</t>
   </si>
+  <si>
+    <t>enumerated</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>hh:mm:ss</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -366,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -404,6 +414,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -625,7 +641,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -712,7 +728,7 @@
         <v>83</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>44</v>
@@ -766,10 +782,16 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="5"/>
+      <c r="J3" s="5" t="s">
+        <v>91</v>
+      </c>
       <c r="K3" s="6"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="3"/>
+      <c r="L3" s="17">
+        <v>36259</v>
+      </c>
+      <c r="M3" s="17">
+        <v>44099</v>
+      </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -932,7 +954,7 @@
         <v>83</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>44</v>
@@ -986,10 +1008,16 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="5"/>
+      <c r="J8" s="5" t="s">
+        <v>92</v>
+      </c>
       <c r="K8" s="6"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="3"/>
+      <c r="L8" s="18">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="M8" s="18">
+        <v>0.98611111111111116</v>
+      </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -1024,10 +1052,16 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="5"/>
+      <c r="J9" s="5" t="s">
+        <v>92</v>
+      </c>
       <c r="K9" s="6"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="3"/>
+      <c r="L9" s="18">
+        <v>5.0694444444444445E-2</v>
+      </c>
+      <c r="M9" s="18">
+        <v>0.66111111111111109</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -1170,7 +1204,7 @@
         <v>83</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>15</v>
@@ -1261,8 +1295,8 @@
       <c r="F15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>85</v>
+      <c r="G15" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>17</v>
@@ -1910,7 +1944,7 @@
         <v>15</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>17</v>
@@ -1952,13 +1986,13 @@
         <v>83</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
checks metadata field errors, validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_snorkel_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\edi-feather-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED5C50C-44B4-4CA6-8ABC-8DC142114FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4476E239-08C6-48A5-89A1-49408A962E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26625" yWindow="1080" windowWidth="19080" windowHeight="14310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="92">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -89,12 +89,6 @@
   </si>
   <si>
     <t>attribute_name</t>
-  </si>
-  <si>
-    <t>ProjectDescriptionID</t>
-  </si>
-  <si>
-    <t>Feather River RST program</t>
   </si>
   <si>
     <t xml:space="preserve">survey_id           </t>
@@ -271,9 +265,6 @@
     <t>Number of map section from DMP</t>
   </si>
   <si>
-    <t>Fish size classification</t>
-  </si>
-  <si>
     <t>ordinal</t>
   </si>
   <si>
@@ -295,16 +286,22 @@
     <t>FNU</t>
   </si>
   <si>
-    <t>none</t>
+    <t>YYYY-MM-DD</t>
   </si>
   <si>
     <t>enumerated</t>
   </si>
   <si>
-    <t>YYYY-MM-DD</t>
+    <t>Fish size classification. Levels = c("III" "I"   NA    "II"  "VI"  "IV"  "V"   "VII")</t>
   </si>
   <si>
     <t>hh:mm:ss</t>
+  </si>
+  <si>
+    <t>survey_id</t>
+  </si>
+  <si>
+    <t>Feather River Snorkel Survey</t>
   </si>
 </sst>
 </file>
@@ -376,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -421,6 +418,9 @@
     </xf>
     <xf numFmtId="21" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -639,9 +639,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -716,38 +716,28 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>57</v>
-      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
       <c r="I2" s="2"/>
       <c r="J2" s="5"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="3">
-        <v>2</v>
-      </c>
-      <c r="M2" s="3">
-        <v>581</v>
-      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -764,26 +754,26 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="2"/>
       <c r="J3" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="K3" s="6"/>
       <c r="L3" s="17">
@@ -808,16 +798,16 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>16</v>
@@ -826,7 +816,7 @@
         <v>15</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>17</v>
@@ -856,16 +846,16 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -894,16 +884,16 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>16</v>
@@ -912,7 +902,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>17</v>
@@ -942,25 +932,25 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>17</v>
@@ -990,26 +980,26 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="2"/>
       <c r="J8" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="18">
@@ -1034,26 +1024,26 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="2"/>
       <c r="J9" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="18">
@@ -1078,16 +1068,16 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>14</v>
@@ -1116,16 +1106,16 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>14</v>
@@ -1154,16 +1144,16 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>14</v>
@@ -1192,28 +1182,28 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="5"/>
@@ -1240,16 +1230,16 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>14</v>
@@ -1278,16 +1268,16 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>16</v>
@@ -1296,7 +1286,7 @@
         <v>15</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>17</v>
@@ -1326,16 +1316,16 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>14</v>
@@ -1364,16 +1354,16 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>14</v>
@@ -1402,16 +1392,16 @@
     </row>
     <row r="18" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>14</v>
@@ -1440,16 +1430,16 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>16</v>
@@ -1458,7 +1448,7 @@
         <v>15</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>17</v>
@@ -1488,16 +1478,16 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>14</v>
@@ -1526,16 +1516,16 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>14</v>
@@ -1564,16 +1554,16 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>14</v>
@@ -1602,16 +1592,16 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>14</v>
@@ -1640,16 +1630,16 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>14</v>
@@ -1678,16 +1668,16 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>14</v>
@@ -1716,16 +1706,16 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>14</v>
@@ -1754,16 +1744,16 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>14</v>
@@ -1792,16 +1782,16 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>16</v>
@@ -1810,10 +1800,10 @@
         <v>15</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="3"/>
@@ -1840,16 +1830,16 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>16</v>
@@ -1858,7 +1848,7 @@
         <v>15</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>17</v>
@@ -1888,16 +1878,16 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>14</v>
@@ -1926,16 +1916,16 @@
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>16</v>
@@ -1944,7 +1934,7 @@
         <v>15</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>17</v>
@@ -1974,38 +1964,28 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>15</v>
+      <c r="E32" s="1" t="s">
+        <v>87</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>57</v>
-      </c>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
       <c r="I32" s="2"/>
       <c r="J32" s="3"/>
       <c r="K32" s="2"/>
-      <c r="L32" s="14">
-        <v>1</v>
-      </c>
-      <c r="M32" s="14">
-        <v>20</v>
-      </c>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
@@ -29247,7 +29227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -29298,10 +29278,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -29328,9 +29308,15 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="8"/>
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>70</v>
+      </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>

</xml_diff>

<commit_message>
changes Turbidity units to NTU
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_snorkel_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\edi-feather-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4476E239-08C6-48A5-89A1-49408A962E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E39DDB1-A9A9-4980-8A29-68039C7DAAE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26625" yWindow="1080" windowWidth="19080" windowHeight="14310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="2180" windowWidth="21580" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -283,9 +283,6 @@
     <t>integer</t>
   </si>
   <si>
-    <t>FNU</t>
-  </si>
-  <si>
     <t>YYYY-MM-DD</t>
   </si>
   <si>
@@ -302,6 +299,9 @@
   </si>
   <si>
     <t>Feather River Snorkel Survey</t>
+  </si>
+  <si>
+    <t>NTU</t>
   </si>
 </sst>
 </file>
@@ -639,9 +639,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -728,7 +728,7 @@
         <v>80</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="3"/>
@@ -773,7 +773,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="2"/>
       <c r="J3" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K3" s="6"/>
       <c r="L3" s="17">
@@ -902,7 +902,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>17</v>
@@ -999,7 +999,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="2"/>
       <c r="J8" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="18">
@@ -1043,7 +1043,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="2"/>
       <c r="J9" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="18">
@@ -1233,7 +1233,7 @@
         <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -1934,7 +1934,7 @@
         <v>15</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>17</v>
@@ -1976,7 +1976,7 @@
         <v>80</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -29227,7 +29227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -29278,10 +29278,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -29312,7 +29312,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
adds possible options in categorical variables
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_snorkel_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\edi-feather-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E39DDB1-A9A9-4980-8A29-68039C7DAAE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C2428A-D462-4862-B07C-E5138607A7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="2180" windowWidth="21580" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7160" yWindow="0" windowWidth="18530" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="93">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -166,25 +166,10 @@
     <t>Date snorkel data was collected</t>
   </si>
   <si>
-    <t>Weather conditions when data was collected (CLD, CLR, RAN)</t>
-  </si>
-  <si>
     <t>Turbidity measured at survey</t>
   </si>
   <si>
     <t xml:space="preserve">Substrate description from survey location </t>
-  </si>
-  <si>
-    <t>Features of stream</t>
-  </si>
-  <si>
-    <t>Run type of the fish counted</t>
-  </si>
-  <si>
-    <t>If fish was tagged or not</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If fish fin is clipped </t>
   </si>
   <si>
     <t>Time when snorkel survey started</t>
@@ -244,9 +229,6 @@
     <t>dateTime</t>
   </si>
   <si>
-    <t>Fish species</t>
-  </si>
-  <si>
     <t>Fork length of juvenile</t>
   </si>
   <si>
@@ -302,6 +284,28 @@
   </si>
   <si>
     <t>NTU</t>
+  </si>
+  <si>
+    <t>Location were snorkel data was collected. Levels = c(Hatchery Riffle, G95, Mo's Ditch, 
+Bedrock Park Riffle, Trailer Park Riffle, Aleck Riffle, Steep Riffle, Eye Riffle, Big Riffle, Vance Riffle, McFarland, Junkyard Riffle, Gateway Riffle, Hatchery Ditch, Matthews Riffle, Gridley Riffle, Robinson Riffle, Kiester Riffle, Goose Riffle, Hatchery and Mo's Riffles, Auditorium Riffle, Hatchery Ditch and Mo's Ditch)</t>
+  </si>
+  <si>
+    <t>Weather conditions when data was collected. Levels = c(clear, sunny, clear and windy, cloudy, partly cloudy, precipitation, hazy, windy, clear and hot, overcast)</t>
+  </si>
+  <si>
+    <t>Features of stream. Levels = c(riffle, glide, glide edgewater, riffle edgewater, backwater, pool)</t>
+  </si>
+  <si>
+    <t>Run type of the fish counted. Levels = c(unknown, spring, fall, late fall)</t>
+  </si>
+  <si>
+    <t>If fish was tagged or not. Levels = c(TRUE, FALSE)</t>
+  </si>
+  <si>
+    <t>If fish fin is clipped. Levels = c(TRUE, FALSE)</t>
+  </si>
+  <si>
+    <t>Fish species. Levels = c(chinook, unknown)</t>
   </si>
 </sst>
 </file>
@@ -640,8 +644,8 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -719,16 +723,16 @@
         <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="3"/>
@@ -760,20 +764,20 @@
         <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="2"/>
       <c r="J3" s="5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K3" s="6"/>
       <c r="L3" s="17">
@@ -807,7 +811,7 @@
         <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>16</v>
@@ -816,7 +820,7 @@
         <v>15</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>17</v>
@@ -846,16 +850,16 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -887,13 +891,13 @@
         <v>24</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>16</v>
@@ -902,7 +906,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>17</v>
@@ -941,7 +945,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
@@ -983,23 +987,23 @@
         <v>26</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="2"/>
       <c r="J8" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="18">
@@ -1027,23 +1031,23 @@
         <v>27</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="2"/>
       <c r="J9" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="18">
@@ -1070,14 +1074,14 @@
       <c r="A10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>59</v>
+      <c r="B10" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>14</v>
@@ -1109,13 +1113,13 @@
         <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>14</v>
@@ -1147,13 +1151,13 @@
         <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>14</v>
@@ -1185,13 +1189,13 @@
         <v>31</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>16</v>
@@ -1200,10 +1204,10 @@
         <v>15</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="5"/>
@@ -1233,13 +1237,13 @@
         <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>14</v>
@@ -1271,13 +1275,13 @@
         <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>16</v>
@@ -1286,7 +1290,7 @@
         <v>15</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>17</v>
@@ -1319,13 +1323,13 @@
         <v>34</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>14</v>
@@ -1357,13 +1361,13 @@
         <v>35</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>14</v>
@@ -1392,16 +1396,16 @@
     </row>
     <row r="18" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>14</v>
@@ -1433,13 +1437,13 @@
         <v>37</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>16</v>
@@ -1448,7 +1452,7 @@
         <v>15</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>17</v>
@@ -1481,13 +1485,13 @@
         <v>38</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>14</v>
@@ -1519,13 +1523,13 @@
         <v>39</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>14</v>
@@ -1557,13 +1561,13 @@
         <v>40</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>14</v>
@@ -1595,13 +1599,13 @@
         <v>36</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>14</v>
@@ -1630,16 +1634,16 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>14</v>
@@ -1668,16 +1672,16 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>14</v>
@@ -1706,16 +1710,16 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>14</v>
@@ -1744,16 +1748,16 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>14</v>
@@ -1782,16 +1786,16 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>16</v>
@@ -1800,10 +1804,10 @@
         <v>15</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="3"/>
@@ -1830,16 +1834,16 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>16</v>
@@ -1848,7 +1852,7 @@
         <v>15</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>17</v>
@@ -1878,16 +1882,16 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>14</v>
@@ -1916,16 +1920,16 @@
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>16</v>
@@ -1934,7 +1938,7 @@
         <v>15</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>17</v>
@@ -1964,19 +1968,19 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -29278,10 +29282,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -29312,10 +29316,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>

</xml_diff>

<commit_message>
adds notes for field reference, validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_snorkel_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\edi-feather-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C2428A-D462-4862-B07C-E5138607A7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388FEEFD-805E-4D4C-BB15-74A79627F6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7160" yWindow="0" windowWidth="18530" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="830" yWindow="1320" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -644,8 +644,8 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
adds definition to units_covered, adds notes/todos
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_snorkel_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\edi-feather-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388FEEFD-805E-4D4C-BB15-74A79627F6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BCB8C6-BDE5-4908-8F7C-0339C497E00F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="830" yWindow="1320" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="94">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -307,6 +307,9 @@
   <si>
     <t>Fish species. Levels = c(chinook, unknown)</t>
   </si>
+  <si>
+    <t xml:space="preserve">Units surveyed within section </t>
+  </si>
 </sst>
 </file>
 
@@ -377,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -425,6 +428,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -645,7 +651,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1112,8 +1118,8 @@
       <c r="A11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>76</v>
+      <c r="B11" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
updates sustrate definition, adds note on md
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_snorkel_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\edi-feather-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BCB8C6-BDE5-4908-8F7C-0339C497E00F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE341F57-411C-44A8-A046-C5B44E709879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,9 +169,6 @@
     <t>Turbidity measured at survey</t>
   </si>
   <si>
-    <t xml:space="preserve">Substrate description from survey location </t>
-  </si>
-  <si>
     <t>Time when snorkel survey started</t>
   </si>
   <si>
@@ -309,6 +306,9 @@
   </si>
   <si>
     <t xml:space="preserve">Units surveyed within section </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substrate code description from survey location </t>
   </si>
 </sst>
 </file>
@@ -650,8 +650,8 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -729,16 +729,16 @@
         <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="3"/>
@@ -770,20 +770,20 @@
         <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="2"/>
       <c r="J3" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K3" s="6"/>
       <c r="L3" s="17">
@@ -817,7 +817,7 @@
         <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>16</v>
@@ -826,7 +826,7 @@
         <v>15</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>17</v>
@@ -856,16 +856,16 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -903,7 +903,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>16</v>
@@ -912,7 +912,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>17</v>
@@ -951,7 +951,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
@@ -993,23 +993,23 @@
         <v>26</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="2"/>
       <c r="J8" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="18">
@@ -1037,23 +1037,23 @@
         <v>27</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="2"/>
       <c r="J9" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="18">
@@ -1081,13 +1081,13 @@
         <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>14</v>
@@ -1119,13 +1119,13 @@
         <v>29</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>14</v>
@@ -1157,13 +1157,13 @@
         <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>14</v>
@@ -1195,13 +1195,13 @@
         <v>31</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>16</v>
@@ -1210,10 +1210,10 @@
         <v>15</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="5"/>
@@ -1243,13 +1243,13 @@
         <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>14</v>
@@ -1281,13 +1281,13 @@
         <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>16</v>
@@ -1296,7 +1296,7 @@
         <v>15</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>17</v>
@@ -1329,13 +1329,13 @@
         <v>34</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>14</v>
@@ -1367,13 +1367,13 @@
         <v>35</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>14</v>
@@ -1402,16 +1402,16 @@
     </row>
     <row r="18" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>14</v>
@@ -1443,13 +1443,13 @@
         <v>37</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>16</v>
@@ -1458,7 +1458,7 @@
         <v>15</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>17</v>
@@ -1491,13 +1491,13 @@
         <v>38</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>14</v>
@@ -1529,13 +1529,13 @@
         <v>39</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>14</v>
@@ -1567,13 +1567,13 @@
         <v>40</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>14</v>
@@ -1605,13 +1605,13 @@
         <v>36</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>14</v>
@@ -1640,16 +1640,16 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>14</v>
@@ -1678,16 +1678,16 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>14</v>
@@ -1716,16 +1716,16 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>14</v>
@@ -1754,16 +1754,16 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>14</v>
@@ -1792,16 +1792,16 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>16</v>
@@ -1810,10 +1810,10 @@
         <v>15</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="3"/>
@@ -1840,16 +1840,16 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>16</v>
@@ -1858,7 +1858,7 @@
         <v>15</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>17</v>
@@ -1888,16 +1888,16 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>14</v>
@@ -1926,16 +1926,16 @@
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>16</v>
@@ -1944,7 +1944,7 @@
         <v>15</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>17</v>
@@ -1974,19 +1974,19 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="E32" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -29288,10 +29288,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -29322,10 +29322,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>

</xml_diff>

<commit_message>
updaes definition of section name and instream cover
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_snorkel_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\edi-feather-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE341F57-411C-44A8-A046-C5B44E709879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F13530-F8A8-4743-BD91-0A7126FD2B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -178,9 +178,6 @@
     <t>whole</t>
   </si>
   <si>
-    <t xml:space="preserve">Instream cover at survey location </t>
-  </si>
-  <si>
     <t>Overhead cover at survey location</t>
   </si>
   <si>
@@ -308,7 +305,10 @@
     <t xml:space="preserve">Units surveyed within section </t>
   </si>
   <si>
-    <t xml:space="preserve">Substrate code description from survey location </t>
+    <t>Substrate code description from survey location. Levels = c( 1- Fine, 2- Small/medium gravel, 3- Medium/large cobble, 4- Boulder, 5- Pavement)</t>
+  </si>
+  <si>
+    <t>Instream cover at survey location. Levels = c(G- Glide, GM- Glide Edgewater, M- Riffle Margin Eddy, P- Pool, R- Riffle, RM- Riffle Edgewater, W- Backwater)</t>
   </si>
 </sst>
 </file>
@@ -651,7 +651,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -729,16 +729,16 @@
         <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="3"/>
@@ -770,20 +770,20 @@
         <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="2"/>
       <c r="J3" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K3" s="6"/>
       <c r="L3" s="17">
@@ -817,7 +817,7 @@
         <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>16</v>
@@ -826,7 +826,7 @@
         <v>15</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>17</v>
@@ -856,16 +856,16 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -903,7 +903,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>16</v>
@@ -912,7 +912,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>17</v>
@@ -951,7 +951,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
@@ -996,20 +996,20 @@
         <v>47</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="2"/>
       <c r="J8" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="18">
@@ -1040,20 +1040,20 @@
         <v>47</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="2"/>
       <c r="J9" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="18">
@@ -1081,13 +1081,13 @@
         <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>14</v>
@@ -1119,13 +1119,13 @@
         <v>29</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>14</v>
@@ -1157,13 +1157,13 @@
         <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>14</v>
@@ -1201,7 +1201,7 @@
         <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>16</v>
@@ -1210,10 +1210,10 @@
         <v>15</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="5"/>
@@ -1243,13 +1243,13 @@
         <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>14</v>
@@ -1281,13 +1281,13 @@
         <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>16</v>
@@ -1296,7 +1296,7 @@
         <v>15</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>17</v>
@@ -1329,13 +1329,13 @@
         <v>34</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>14</v>
@@ -1367,13 +1367,13 @@
         <v>35</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>14</v>
@@ -1402,16 +1402,16 @@
     </row>
     <row r="18" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>14</v>
@@ -1443,13 +1443,13 @@
         <v>37</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>16</v>
@@ -1458,7 +1458,7 @@
         <v>15</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>17</v>
@@ -1491,13 +1491,13 @@
         <v>38</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>14</v>
@@ -1529,13 +1529,13 @@
         <v>39</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>14</v>
@@ -1567,13 +1567,13 @@
         <v>40</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>14</v>
@@ -1605,13 +1605,13 @@
         <v>36</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>14</v>
@@ -1640,16 +1640,16 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>14</v>
@@ -1678,16 +1678,16 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>14</v>
@@ -1716,16 +1716,16 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>14</v>
@@ -1754,16 +1754,16 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>14</v>
@@ -1792,16 +1792,16 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>16</v>
@@ -1810,7 +1810,7 @@
         <v>15</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>49</v>
@@ -1840,16 +1840,16 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>16</v>
@@ -1858,7 +1858,7 @@
         <v>15</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>17</v>
@@ -1888,16 +1888,16 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>14</v>
@@ -1926,16 +1926,16 @@
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>16</v>
@@ -1944,7 +1944,7 @@
         <v>15</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>17</v>
@@ -1974,19 +1974,19 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="E32" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -29288,10 +29288,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -29322,10 +29322,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>

</xml_diff>

<commit_message>
modifies field definitions according to team's clarification
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_snorkel_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\edi-feather-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F13530-F8A8-4743-BD91-0A7126FD2B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD858888-C617-4122-B2D6-3C13A8BDEA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="97">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -229,9 +229,6 @@
     <t>millimeter</t>
   </si>
   <si>
-    <t>Distance from the bank</t>
-  </si>
-  <si>
     <t>meter</t>
   </si>
   <si>
@@ -309,6 +306,18 @@
   </si>
   <si>
     <t>Instream cover at survey location. Levels = c(G- Glide, GM- Glide Edgewater, M- Riffle Margin Eddy, P- Pool, R- Riffle, RM- Riffle Edgewater, W- Backwater)</t>
+  </si>
+  <si>
+    <t>Distance from the bank from observation</t>
+  </si>
+  <si>
+    <t>Visibility range that allows to identify fish</t>
+  </si>
+  <si>
+    <t>Estimated fork length of observed fish</t>
+  </si>
+  <si>
+    <t>Survey site type. Levels = c(Permanent: site surveyed repetedly, Random = site surveyed as a proxy if "permanent site" not feasible to survey)</t>
   </si>
 </sst>
 </file>
@@ -650,8 +659,8 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -729,16 +738,16 @@
         <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="3"/>
@@ -773,7 +782,7 @@
         <v>64</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>64</v>
@@ -783,7 +792,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="2"/>
       <c r="J3" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K3" s="6"/>
       <c r="L3" s="17">
@@ -817,7 +826,7 @@
         <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>16</v>
@@ -826,7 +835,7 @@
         <v>15</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>17</v>
@@ -859,13 +868,13 @@
         <v>53</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -903,7 +912,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>16</v>
@@ -912,7 +921,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>17</v>
@@ -951,7 +960,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
@@ -999,7 +1008,7 @@
         <v>64</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>64</v>
@@ -1009,7 +1018,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="2"/>
       <c r="J8" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="18">
@@ -1043,7 +1052,7 @@
         <v>64</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>64</v>
@@ -1053,7 +1062,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="2"/>
       <c r="J9" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="18">
@@ -1081,13 +1090,13 @@
         <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>14</v>
@@ -1119,13 +1128,13 @@
         <v>29</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>14</v>
@@ -1157,13 +1166,13 @@
         <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>14</v>
@@ -1201,7 +1210,7 @@
         <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>16</v>
@@ -1210,10 +1219,10 @@
         <v>15</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="5"/>
@@ -1243,13 +1252,13 @@
         <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>14</v>
@@ -1281,13 +1290,13 @@
         <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>16</v>
@@ -1329,13 +1338,13 @@
         <v>34</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>14</v>
@@ -1367,13 +1376,13 @@
         <v>35</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>14</v>
@@ -1405,13 +1414,13 @@
         <v>54</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>14</v>
@@ -1449,7 +1458,7 @@
         <v>15</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>16</v>
@@ -1458,7 +1467,7 @@
         <v>15</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>17</v>
@@ -1491,13 +1500,13 @@
         <v>38</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>14</v>
@@ -1529,13 +1538,13 @@
         <v>39</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>14</v>
@@ -1567,13 +1576,13 @@
         <v>40</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>14</v>
@@ -1611,7 +1620,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>14</v>
@@ -1649,7 +1658,7 @@
         <v>13</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>14</v>
@@ -1681,13 +1690,13 @@
         <v>56</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>14</v>
@@ -1719,13 +1728,13 @@
         <v>57</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>14</v>
@@ -1757,13 +1766,13 @@
         <v>58</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>14</v>
@@ -1801,7 +1810,7 @@
         <v>15</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>16</v>
@@ -1843,13 +1852,13 @@
         <v>60</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>16</v>
@@ -1858,7 +1867,7 @@
         <v>15</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>17</v>
@@ -1891,13 +1900,13 @@
         <v>61</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>14</v>
@@ -1929,13 +1938,13 @@
         <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>16</v>
@@ -1944,7 +1953,7 @@
         <v>15</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>17</v>
@@ -1977,16 +1986,16 @@
         <v>63</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="E32" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -29288,10 +29297,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -29322,7 +29331,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
updates clean data to include notes and action items after converstaion with Casey
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_snorkel_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erincain/Documents/Git/edi-feather-snorkel/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B46FE48-BBC9-5141-AE2A-921170D00945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBB06CB-ED8F-F14F-A945-0CF8127594B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-6840" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="95">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -235,9 +235,6 @@
     <t>YYYY-MM-DD</t>
   </si>
   <si>
-    <t>enumerated</t>
-  </si>
-  <si>
     <t>hh:mm:ss</t>
   </si>
   <si>
@@ -245,18 +242,6 @@
   </si>
   <si>
     <t>Estimated fork length of observed fish</t>
-  </si>
-  <si>
-    <t>Weather conditions when data was collected. Weather conditions include = c("clear", "sunny", "clear and windy", "cloudy", "partly cloudy", "precipitation", "hazy", "windy", "clear and hot", "overcast")</t>
-  </si>
-  <si>
-    <t>Fish size classification. Classification = c("III" "I"   NA    "II"  "VI"  "IV"  "V"   "VII")</t>
-  </si>
-  <si>
-    <t>Run type of the fish counted. Types of run include = c(unknown, spring, fall, late fall)</t>
-  </si>
-  <si>
-    <t>Survey site type. Site types include = c(Permanent: site surveyed repetedly, Random = site surveyed as a proxy if "permanent site" not feasible to survey)</t>
   </si>
   <si>
     <t>Flow in cubic feet per seccond (cfs)</t>
@@ -277,12 +262,6 @@
     <t>Substrate code description from survey location. If multiple substrates are observed at one site, all substrate types are reccorded. Levels = c( 1- Fine, 2- Small/medium gravel, 3- Medium/large cobble, 4- Boulder, 5- Pavement)</t>
   </si>
   <si>
-    <t>Instream cover at survey location. If multiple cover types are observed at one site, all cover types are reccorded. Types of cover include = c()</t>
-  </si>
-  <si>
-    <t>Hydological features at study site. Features include = c(riffle, glide, glide edgewater, riffle edgewater, backwater, pool)</t>
-  </si>
-  <si>
     <t>Depth of water in meters</t>
   </si>
   <si>
@@ -290,9 +269,6 @@
   </si>
   <si>
     <t>If fish was tagged or not (TRUE, FALSE)</t>
-  </si>
-  <si>
-    <t>Overhead cover at survey location.  If multiple cover types are observed at one site, all cover types are reccorded. Types of cover include = c()</t>
   </si>
   <si>
     <t>Location where snorkel data is collected</t>
@@ -313,7 +289,28 @@
     <t xml:space="preserve">Distance under current conditions of how far you can see/identify a fish. Recorded in meters. </t>
   </si>
   <si>
-    <t>Number corresponding to section name. TODO list source</t>
+    <t>Fish size classification. Classification types include: III, I,  NA , II, VI, IV, V, VII</t>
+  </si>
+  <si>
+    <t>Weather conditions when data was collected. Weather conditions include: clear, sunny, clear and windy, cloudy, partly cloudy, precipitation, hazy, windy, clear and hot, overcast</t>
+  </si>
+  <si>
+    <t>Hydological features at study site. Features include: riffle, glide, glide edgewater, riffle edgewater, backwater, pool)</t>
+  </si>
+  <si>
+    <t>Run type of the fish counted. Types of run include: unknown, spring, fall, late fall</t>
+  </si>
+  <si>
+    <t>Survey site type. Site types include: permanent - site surveyed repetedly, Random - site surveyed as a proxy if "permanent site" not feasible to survey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instream cover at survey location. If multiple cover types are observed at one site, all cover types are reccorded. Types of cover include: E - Submerged Aquatic Veg/Algae, B - Small Instream Objects/Woody Debris, C - Large Instream Objects/Woody Debris, A - No apparent Cover, F - undercut bank </t>
+  </si>
+  <si>
+    <t>Overhead cover at survey location.  If multiple cover types are observed at one site, all cover types are reccorded. Types of cover include: 0 - no apparent cover, 1 - overhead object/veg 0 - 0.5 meters, 2 - overhead object/veg 0.5 - 2 meters, 3 - submerged aquatic veg/algae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number corresponding to section name. </t>
   </si>
 </sst>
 </file>
@@ -660,9 +657,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -750,7 +747,7 @@
         <v>64</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="3"/>
@@ -823,7 +820,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>41</v>
@@ -871,7 +868,7 @@
         <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -924,7 +921,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>17</v>
@@ -1021,7 +1018,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="2"/>
       <c r="J8" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="18">
@@ -1049,7 +1046,7 @@
         <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>59</v>
@@ -1065,7 +1062,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="2"/>
       <c r="J9" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="18">
@@ -1093,7 +1090,7 @@
         <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
@@ -1131,7 +1128,7 @@
         <v>29</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
@@ -1169,7 +1166,7 @@
         <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
@@ -1255,7 +1252,7 @@
         <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -1293,7 +1290,7 @@
         <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
@@ -1341,7 +1338,7 @@
         <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -1379,7 +1376,7 @@
         <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -1417,7 +1414,7 @@
         <v>50</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
@@ -1455,7 +1452,7 @@
         <v>37</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>15</v>
@@ -1503,7 +1500,7 @@
         <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>13</v>
@@ -1541,7 +1538,7 @@
         <v>39</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>13</v>
@@ -1579,7 +1576,7 @@
         <v>40</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>13</v>
@@ -1617,7 +1614,7 @@
         <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>13</v>
@@ -1655,7 +1652,7 @@
         <v>51</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>13</v>
@@ -1693,7 +1690,7 @@
         <v>52</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>13</v>
@@ -1731,7 +1728,7 @@
         <v>53</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>13</v>
@@ -1769,7 +1766,7 @@
         <v>54</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>13</v>
@@ -1807,7 +1804,7 @@
         <v>55</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>15</v>
@@ -1855,7 +1852,7 @@
         <v>56</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>15</v>
@@ -1903,7 +1900,7 @@
         <v>57</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>15</v>
@@ -1951,7 +1948,7 @@
         <v>58</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>63</v>
@@ -1960,7 +1957,7 @@
         <v>64</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -29211,7 +29208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>